<commit_message>
update: remove unusable codes & functions
</commit_message>
<xml_diff>
--- a/frontend/public/assets/template_nilai_IPA.xlsx
+++ b/frontend/public/assets/template_nilai_IPA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamyo\Code Box\srjk\frontend\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamyo\Code Box\srjk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3762A4D4-F442-4A57-8AA5-7DB9E46876BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94E4F85-1FE6-463B-9B47-53EF36F7851B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
   <si>
     <t>NO.</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Ekonomi</t>
   </si>
   <si>
-    <t>Bahasa Inggris</t>
-  </si>
-  <si>
     <t>ANGKATAN</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>JURUSAN</t>
+  </si>
+  <si>
+    <t>RUMPUN JURUSAN</t>
   </si>
 </sst>
 </file>
@@ -477,30 +477,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BY37"/>
+  <dimension ref="A1:BX37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BZ1" sqref="BZ1:BZ1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="5.81640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="32" width="5.26953125" customWidth="1"/>
-    <col min="33" max="46" width="4.7265625" customWidth="1"/>
-    <col min="47" max="60" width="4.26953125" customWidth="1"/>
-    <col min="61" max="74" width="4.54296875" customWidth="1"/>
-    <col min="75" max="75" width="9.1796875"/>
-    <col min="76" max="76" width="43.26953125" style="1" customWidth="1"/>
-    <col min="77" max="77" width="23.81640625" style="1" customWidth="1"/>
-    <col min="78" max="16383" width="9.1796875"/>
-    <col min="16384" max="16384" width="9.1796875" customWidth="1"/>
+    <col min="3" max="30" width="5.26953125" customWidth="1"/>
+    <col min="31" max="44" width="4.7265625" customWidth="1"/>
+    <col min="45" max="58" width="4.26953125" customWidth="1"/>
+    <col min="59" max="72" width="4.54296875" customWidth="1"/>
+    <col min="73" max="73" width="9.1796875"/>
+    <col min="74" max="74" width="43.26953125" style="1" customWidth="1"/>
+    <col min="75" max="75" width="23.81640625" style="1" customWidth="1"/>
+    <col min="76" max="76" width="28.81640625" style="1" customWidth="1"/>
+    <col min="77" max="16382" width="9.1796875"/>
+    <col min="16383" max="16384" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="12" customHeight="1"/>
-    <row r="2" spans="1:77" ht="12.5"/>
-    <row r="3" spans="1:77" ht="12.5">
+    <row r="1" spans="1:76" ht="12" customHeight="1"/>
+    <row r="2" spans="1:76" ht="12.5"/>
+    <row r="3" spans="1:76" ht="12.5">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -523,10 +524,10 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
@@ -539,11 +540,11 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
       <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
+      <c r="AE3" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="AF3" s="12"/>
-      <c r="AG3" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="12"/>
       <c r="AJ3" s="12"/>
@@ -555,11 +556,11 @@
       <c r="AP3" s="12"/>
       <c r="AQ3" s="12"/>
       <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
+      <c r="AS3" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="AT3" s="12"/>
-      <c r="AU3" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="AU3" s="12"/>
       <c r="AV3" s="12"/>
       <c r="AW3" s="12"/>
       <c r="AX3" s="12"/>
@@ -571,11 +572,11 @@
       <c r="BD3" s="12"/>
       <c r="BE3" s="12"/>
       <c r="BF3" s="12"/>
-      <c r="BG3" s="12"/>
+      <c r="BG3" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="BH3" s="12"/>
-      <c r="BI3" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="BI3" s="12"/>
       <c r="BJ3" s="12"/>
       <c r="BK3" s="12"/>
       <c r="BL3" s="12"/>
@@ -587,13 +588,12 @@
       <c r="BR3" s="12"/>
       <c r="BS3" s="12"/>
       <c r="BT3" s="12"/>
-      <c r="BU3" s="12"/>
-      <c r="BV3" s="12"/>
-      <c r="BW3" s="9"/>
+      <c r="BU3" s="9"/>
+      <c r="BV3" s="10"/>
+      <c r="BW3" s="10"/>
       <c r="BX3" s="10"/>
-      <c r="BY3" s="10"/>
     </row>
-    <row r="4" spans="1:77" ht="77">
+    <row r="4" spans="1:76" ht="73.5">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="3" t="s">
@@ -638,191 +638,188 @@
       <c r="P4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AY4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="BI4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BL4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BM4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BP4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BQ4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="BS4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="BT4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="BU4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AO4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AS4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AT4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="BA4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="BB4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="BC4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="BD4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="BE4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="BG4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="BH4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="BK4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="BM4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BN4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="BO4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="BP4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="BR4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="BS4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="BT4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="BU4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="BV4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="BW4" s="7" t="s">
+      <c r="BV4" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="BW4" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="BX4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="BY4" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:77" ht="12.5">
+    <row r="5" spans="1:76" ht="12.5">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
@@ -895,13 +892,12 @@
       <c r="BR5" s="2"/>
       <c r="BS5" s="2"/>
       <c r="BT5" s="2"/>
-      <c r="BU5" s="2"/>
-      <c r="BV5" s="2"/>
-      <c r="BW5" s="9"/>
+      <c r="BU5" s="9"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="10"/>
       <c r="BX5" s="10"/>
-      <c r="BY5" s="10"/>
     </row>
-    <row r="6" spans="1:77" ht="12.5">
+    <row r="6" spans="1:76" ht="12.5">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="2"/>
@@ -974,13 +970,12 @@
       <c r="BR6" s="2"/>
       <c r="BS6" s="2"/>
       <c r="BT6" s="2"/>
-      <c r="BU6" s="2"/>
-      <c r="BV6" s="2"/>
-      <c r="BW6" s="9"/>
+      <c r="BU6" s="9"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
       <c r="BX6" s="10"/>
-      <c r="BY6" s="10"/>
     </row>
-    <row r="7" spans="1:77" ht="12.5">
+    <row r="7" spans="1:76" ht="12.5">
       <c r="A7" s="2"/>
       <c r="B7" s="5"/>
       <c r="C7" s="2"/>
@@ -1053,13 +1048,12 @@
       <c r="BR7" s="2"/>
       <c r="BS7" s="2"/>
       <c r="BT7" s="2"/>
-      <c r="BU7" s="2"/>
-      <c r="BV7" s="2"/>
-      <c r="BW7" s="9"/>
+      <c r="BU7" s="9"/>
+      <c r="BV7" s="10"/>
+      <c r="BW7" s="10"/>
       <c r="BX7" s="10"/>
-      <c r="BY7" s="10"/>
     </row>
-    <row r="8" spans="1:77" ht="12.5">
+    <row r="8" spans="1:76" ht="12.5">
       <c r="A8" s="2"/>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
@@ -1132,13 +1126,12 @@
       <c r="BR8" s="2"/>
       <c r="BS8" s="2"/>
       <c r="BT8" s="2"/>
-      <c r="BU8" s="2"/>
-      <c r="BV8" s="2"/>
-      <c r="BW8" s="9"/>
+      <c r="BU8" s="9"/>
+      <c r="BV8" s="10"/>
+      <c r="BW8" s="10"/>
       <c r="BX8" s="10"/>
-      <c r="BY8" s="10"/>
     </row>
-    <row r="9" spans="1:77" ht="12.5">
+    <row r="9" spans="1:76" ht="12.5">
       <c r="A9" s="2"/>
       <c r="B9" s="5"/>
       <c r="C9" s="2"/>
@@ -1211,13 +1204,12 @@
       <c r="BR9" s="2"/>
       <c r="BS9" s="2"/>
       <c r="BT9" s="2"/>
-      <c r="BU9" s="2"/>
-      <c r="BV9" s="2"/>
-      <c r="BW9" s="9"/>
+      <c r="BU9" s="9"/>
+      <c r="BV9" s="10"/>
+      <c r="BW9" s="10"/>
       <c r="BX9" s="10"/>
-      <c r="BY9" s="10"/>
     </row>
-    <row r="10" spans="1:77" ht="12.5">
+    <row r="10" spans="1:76" ht="12.5">
       <c r="A10" s="2"/>
       <c r="B10" s="5"/>
       <c r="C10" s="2"/>
@@ -1290,13 +1282,12 @@
       <c r="BR10" s="2"/>
       <c r="BS10" s="2"/>
       <c r="BT10" s="2"/>
-      <c r="BU10" s="2"/>
-      <c r="BV10" s="2"/>
-      <c r="BW10" s="9"/>
+      <c r="BU10" s="9"/>
+      <c r="BV10" s="10"/>
+      <c r="BW10" s="10"/>
       <c r="BX10" s="10"/>
-      <c r="BY10" s="10"/>
     </row>
-    <row r="11" spans="1:77" ht="12.5">
+    <row r="11" spans="1:76" ht="12.5">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="2"/>
@@ -1369,13 +1360,12 @@
       <c r="BR11" s="2"/>
       <c r="BS11" s="2"/>
       <c r="BT11" s="2"/>
-      <c r="BU11" s="2"/>
-      <c r="BV11" s="2"/>
-      <c r="BW11" s="9"/>
+      <c r="BU11" s="9"/>
+      <c r="BV11" s="10"/>
+      <c r="BW11" s="10"/>
       <c r="BX11" s="10"/>
-      <c r="BY11" s="10"/>
     </row>
-    <row r="12" spans="1:77" ht="12.5">
+    <row r="12" spans="1:76" ht="12.5">
       <c r="A12" s="2"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2"/>
@@ -1448,13 +1438,12 @@
       <c r="BR12" s="2"/>
       <c r="BS12" s="2"/>
       <c r="BT12" s="2"/>
-      <c r="BU12" s="2"/>
-      <c r="BV12" s="2"/>
-      <c r="BW12" s="9"/>
+      <c r="BU12" s="9"/>
+      <c r="BV12" s="10"/>
+      <c r="BW12" s="10"/>
       <c r="BX12" s="10"/>
-      <c r="BY12" s="10"/>
     </row>
-    <row r="13" spans="1:77" ht="12.5">
+    <row r="13" spans="1:76" ht="12.5">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
       <c r="C13" s="2"/>
@@ -1527,13 +1516,12 @@
       <c r="BR13" s="2"/>
       <c r="BS13" s="2"/>
       <c r="BT13" s="2"/>
-      <c r="BU13" s="2"/>
-      <c r="BV13" s="2"/>
-      <c r="BW13" s="9"/>
+      <c r="BU13" s="9"/>
+      <c r="BV13" s="10"/>
+      <c r="BW13" s="10"/>
       <c r="BX13" s="10"/>
-      <c r="BY13" s="10"/>
     </row>
-    <row r="14" spans="1:77" ht="12.5">
+    <row r="14" spans="1:76" ht="12.5">
       <c r="A14" s="2"/>
       <c r="B14" s="5"/>
       <c r="C14" s="2"/>
@@ -1606,13 +1594,12 @@
       <c r="BR14" s="2"/>
       <c r="BS14" s="2"/>
       <c r="BT14" s="2"/>
-      <c r="BU14" s="2"/>
-      <c r="BV14" s="2"/>
-      <c r="BW14" s="9"/>
+      <c r="BU14" s="9"/>
+      <c r="BV14" s="10"/>
+      <c r="BW14" s="10"/>
       <c r="BX14" s="10"/>
-      <c r="BY14" s="10"/>
     </row>
-    <row r="15" spans="1:77" ht="12.5">
+    <row r="15" spans="1:76" ht="12.5">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
       <c r="C15" s="2"/>
@@ -1685,13 +1672,12 @@
       <c r="BR15" s="2"/>
       <c r="BS15" s="2"/>
       <c r="BT15" s="2"/>
-      <c r="BU15" s="2"/>
-      <c r="BV15" s="2"/>
-      <c r="BW15" s="9"/>
+      <c r="BU15" s="9"/>
+      <c r="BV15" s="10"/>
+      <c r="BW15" s="10"/>
       <c r="BX15" s="10"/>
-      <c r="BY15" s="10"/>
     </row>
-    <row r="16" spans="1:77" ht="12.5">
+    <row r="16" spans="1:76" ht="12.5">
       <c r="A16" s="2"/>
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
@@ -1764,13 +1750,12 @@
       <c r="BR16" s="2"/>
       <c r="BS16" s="2"/>
       <c r="BT16" s="2"/>
-      <c r="BU16" s="2"/>
-      <c r="BV16" s="2"/>
-      <c r="BW16" s="9"/>
+      <c r="BU16" s="9"/>
+      <c r="BV16" s="10"/>
+      <c r="BW16" s="10"/>
       <c r="BX16" s="10"/>
-      <c r="BY16" s="10"/>
     </row>
-    <row r="17" spans="1:77" ht="12.5">
+    <row r="17" spans="1:76" ht="12.5">
       <c r="A17" s="2"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2"/>
@@ -1843,13 +1828,12 @@
       <c r="BR17" s="2"/>
       <c r="BS17" s="2"/>
       <c r="BT17" s="2"/>
-      <c r="BU17" s="2"/>
-      <c r="BV17" s="2"/>
-      <c r="BW17" s="9"/>
+      <c r="BU17" s="9"/>
+      <c r="BV17" s="10"/>
+      <c r="BW17" s="10"/>
       <c r="BX17" s="10"/>
-      <c r="BY17" s="10"/>
     </row>
-    <row r="18" spans="1:77" ht="12.5">
+    <row r="18" spans="1:76" ht="12.5">
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="2"/>
@@ -1922,13 +1906,12 @@
       <c r="BR18" s="2"/>
       <c r="BS18" s="2"/>
       <c r="BT18" s="2"/>
-      <c r="BU18" s="2"/>
-      <c r="BV18" s="2"/>
-      <c r="BW18" s="9"/>
+      <c r="BU18" s="9"/>
+      <c r="BV18" s="10"/>
+      <c r="BW18" s="10"/>
       <c r="BX18" s="10"/>
-      <c r="BY18" s="10"/>
     </row>
-    <row r="19" spans="1:77" ht="12.5">
+    <row r="19" spans="1:76" ht="12.5">
       <c r="A19" s="2"/>
       <c r="B19" s="5"/>
       <c r="C19" s="2"/>
@@ -2001,13 +1984,12 @@
       <c r="BR19" s="2"/>
       <c r="BS19" s="2"/>
       <c r="BT19" s="2"/>
-      <c r="BU19" s="2"/>
-      <c r="BV19" s="2"/>
-      <c r="BW19" s="9"/>
+      <c r="BU19" s="9"/>
+      <c r="BV19" s="10"/>
+      <c r="BW19" s="10"/>
       <c r="BX19" s="10"/>
-      <c r="BY19" s="10"/>
     </row>
-    <row r="20" spans="1:77" ht="12.5">
+    <row r="20" spans="1:76" ht="12.5">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
       <c r="C20" s="2"/>
@@ -2080,13 +2062,12 @@
       <c r="BR20" s="2"/>
       <c r="BS20" s="2"/>
       <c r="BT20" s="2"/>
-      <c r="BU20" s="2"/>
-      <c r="BV20" s="2"/>
-      <c r="BW20" s="9"/>
+      <c r="BU20" s="9"/>
+      <c r="BV20" s="10"/>
+      <c r="BW20" s="10"/>
       <c r="BX20" s="10"/>
-      <c r="BY20" s="10"/>
     </row>
-    <row r="21" spans="1:77" ht="12.5">
+    <row r="21" spans="1:76" ht="12.5">
       <c r="A21" s="2"/>
       <c r="B21" s="5"/>
       <c r="C21" s="2"/>
@@ -2159,13 +2140,12 @@
       <c r="BR21" s="2"/>
       <c r="BS21" s="2"/>
       <c r="BT21" s="2"/>
-      <c r="BU21" s="2"/>
-      <c r="BV21" s="2"/>
-      <c r="BW21" s="9"/>
+      <c r="BU21" s="9"/>
+      <c r="BV21" s="10"/>
+      <c r="BW21" s="10"/>
       <c r="BX21" s="10"/>
-      <c r="BY21" s="10"/>
     </row>
-    <row r="22" spans="1:77" ht="12.5">
+    <row r="22" spans="1:76" ht="12.5">
       <c r="A22" s="2"/>
       <c r="B22" s="5"/>
       <c r="C22" s="2"/>
@@ -2238,13 +2218,12 @@
       <c r="BR22" s="2"/>
       <c r="BS22" s="2"/>
       <c r="BT22" s="2"/>
-      <c r="BU22" s="2"/>
-      <c r="BV22" s="2"/>
-      <c r="BW22" s="9"/>
+      <c r="BU22" s="9"/>
+      <c r="BV22" s="10"/>
+      <c r="BW22" s="10"/>
       <c r="BX22" s="10"/>
-      <c r="BY22" s="10"/>
     </row>
-    <row r="23" spans="1:77" ht="12.5">
+    <row r="23" spans="1:76" ht="12.5">
       <c r="A23" s="2"/>
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
@@ -2317,13 +2296,12 @@
       <c r="BR23" s="2"/>
       <c r="BS23" s="2"/>
       <c r="BT23" s="2"/>
-      <c r="BU23" s="2"/>
-      <c r="BV23" s="2"/>
-      <c r="BW23" s="9"/>
+      <c r="BU23" s="9"/>
+      <c r="BV23" s="10"/>
+      <c r="BW23" s="10"/>
       <c r="BX23" s="10"/>
-      <c r="BY23" s="10"/>
     </row>
-    <row r="24" spans="1:77" ht="12.5">
+    <row r="24" spans="1:76" ht="12.5">
       <c r="A24" s="2"/>
       <c r="B24" s="5"/>
       <c r="C24" s="2"/>
@@ -2396,13 +2374,12 @@
       <c r="BR24" s="2"/>
       <c r="BS24" s="2"/>
       <c r="BT24" s="2"/>
-      <c r="BU24" s="2"/>
-      <c r="BV24" s="2"/>
-      <c r="BW24" s="9"/>
+      <c r="BU24" s="9"/>
+      <c r="BV24" s="10"/>
+      <c r="BW24" s="10"/>
       <c r="BX24" s="10"/>
-      <c r="BY24" s="10"/>
     </row>
-    <row r="25" spans="1:77" ht="12.5">
+    <row r="25" spans="1:76" ht="12.5">
       <c r="A25" s="2"/>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -2475,13 +2452,12 @@
       <c r="BR25" s="2"/>
       <c r="BS25" s="2"/>
       <c r="BT25" s="2"/>
-      <c r="BU25" s="2"/>
-      <c r="BV25" s="2"/>
-      <c r="BW25" s="9"/>
+      <c r="BU25" s="9"/>
+      <c r="BV25" s="10"/>
+      <c r="BW25" s="10"/>
       <c r="BX25" s="10"/>
-      <c r="BY25" s="10"/>
     </row>
-    <row r="26" spans="1:77" ht="12.5">
+    <row r="26" spans="1:76" ht="12.5">
       <c r="A26" s="2"/>
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
@@ -2554,13 +2530,12 @@
       <c r="BR26" s="2"/>
       <c r="BS26" s="2"/>
       <c r="BT26" s="2"/>
-      <c r="BU26" s="2"/>
-      <c r="BV26" s="2"/>
-      <c r="BW26" s="9"/>
+      <c r="BU26" s="9"/>
+      <c r="BV26" s="10"/>
+      <c r="BW26" s="10"/>
       <c r="BX26" s="10"/>
-      <c r="BY26" s="10"/>
     </row>
-    <row r="27" spans="1:77" ht="12.5">
+    <row r="27" spans="1:76" ht="12.5">
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
@@ -2633,13 +2608,12 @@
       <c r="BR27" s="2"/>
       <c r="BS27" s="2"/>
       <c r="BT27" s="2"/>
-      <c r="BU27" s="2"/>
-      <c r="BV27" s="2"/>
-      <c r="BW27" s="9"/>
+      <c r="BU27" s="9"/>
+      <c r="BV27" s="10"/>
+      <c r="BW27" s="10"/>
       <c r="BX27" s="10"/>
-      <c r="BY27" s="10"/>
     </row>
-    <row r="28" spans="1:77" ht="12.5">
+    <row r="28" spans="1:76" ht="12.5">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
@@ -2712,13 +2686,12 @@
       <c r="BR28" s="2"/>
       <c r="BS28" s="2"/>
       <c r="BT28" s="2"/>
-      <c r="BU28" s="2"/>
-      <c r="BV28" s="2"/>
-      <c r="BW28" s="9"/>
+      <c r="BU28" s="9"/>
+      <c r="BV28" s="10"/>
+      <c r="BW28" s="10"/>
       <c r="BX28" s="10"/>
-      <c r="BY28" s="10"/>
     </row>
-    <row r="29" spans="1:77" ht="12.5">
+    <row r="29" spans="1:76" ht="12.5">
       <c r="A29" s="2"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2"/>
@@ -2791,13 +2764,12 @@
       <c r="BR29" s="2"/>
       <c r="BS29" s="2"/>
       <c r="BT29" s="2"/>
-      <c r="BU29" s="2"/>
-      <c r="BV29" s="2"/>
-      <c r="BW29" s="9"/>
+      <c r="BU29" s="9"/>
+      <c r="BV29" s="10"/>
+      <c r="BW29" s="10"/>
       <c r="BX29" s="10"/>
-      <c r="BY29" s="10"/>
     </row>
-    <row r="30" spans="1:77" ht="12.5">
+    <row r="30" spans="1:76" ht="12.5">
       <c r="A30" s="2"/>
       <c r="B30" s="5"/>
       <c r="C30" s="2"/>
@@ -2870,13 +2842,12 @@
       <c r="BR30" s="2"/>
       <c r="BS30" s="2"/>
       <c r="BT30" s="2"/>
-      <c r="BU30" s="2"/>
-      <c r="BV30" s="2"/>
-      <c r="BW30" s="9"/>
+      <c r="BU30" s="9"/>
+      <c r="BV30" s="10"/>
+      <c r="BW30" s="10"/>
       <c r="BX30" s="10"/>
-      <c r="BY30" s="10"/>
     </row>
-    <row r="31" spans="1:77" ht="12.5">
+    <row r="31" spans="1:76" ht="12.5">
       <c r="A31" s="2"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
@@ -2949,13 +2920,12 @@
       <c r="BR31" s="2"/>
       <c r="BS31" s="2"/>
       <c r="BT31" s="2"/>
-      <c r="BU31" s="2"/>
-      <c r="BV31" s="2"/>
-      <c r="BW31" s="9"/>
+      <c r="BU31" s="9"/>
+      <c r="BV31" s="10"/>
+      <c r="BW31" s="10"/>
       <c r="BX31" s="10"/>
-      <c r="BY31" s="10"/>
     </row>
-    <row r="32" spans="1:77" ht="12.5">
+    <row r="32" spans="1:76" ht="12.5">
       <c r="A32" s="2"/>
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
@@ -3028,13 +2998,12 @@
       <c r="BR32" s="2"/>
       <c r="BS32" s="2"/>
       <c r="BT32" s="2"/>
-      <c r="BU32" s="2"/>
-      <c r="BV32" s="2"/>
-      <c r="BW32" s="9"/>
+      <c r="BU32" s="9"/>
+      <c r="BV32" s="10"/>
+      <c r="BW32" s="10"/>
       <c r="BX32" s="10"/>
-      <c r="BY32" s="10"/>
     </row>
-    <row r="33" spans="1:77" ht="12.5">
+    <row r="33" spans="1:76" ht="12.5">
       <c r="A33" s="2"/>
       <c r="B33" s="5"/>
       <c r="C33" s="2"/>
@@ -3107,13 +3076,12 @@
       <c r="BR33" s="2"/>
       <c r="BS33" s="2"/>
       <c r="BT33" s="2"/>
-      <c r="BU33" s="2"/>
-      <c r="BV33" s="2"/>
-      <c r="BW33" s="9"/>
+      <c r="BU33" s="9"/>
+      <c r="BV33" s="10"/>
+      <c r="BW33" s="10"/>
       <c r="BX33" s="10"/>
-      <c r="BY33" s="10"/>
     </row>
-    <row r="34" spans="1:77" ht="12.5">
+    <row r="34" spans="1:76" ht="12.5">
       <c r="A34" s="2"/>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
@@ -3186,13 +3154,12 @@
       <c r="BR34" s="2"/>
       <c r="BS34" s="2"/>
       <c r="BT34" s="2"/>
-      <c r="BU34" s="2"/>
-      <c r="BV34" s="2"/>
-      <c r="BW34" s="9"/>
+      <c r="BU34" s="9"/>
+      <c r="BV34" s="10"/>
+      <c r="BW34" s="10"/>
       <c r="BX34" s="10"/>
-      <c r="BY34" s="10"/>
     </row>
-    <row r="35" spans="1:77" ht="12.5">
+    <row r="35" spans="1:76" ht="12.5">
       <c r="A35" s="2"/>
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
@@ -3265,13 +3232,12 @@
       <c r="BR35" s="2"/>
       <c r="BS35" s="2"/>
       <c r="BT35" s="2"/>
-      <c r="BU35" s="2"/>
-      <c r="BV35" s="2"/>
-      <c r="BW35" s="9"/>
+      <c r="BU35" s="9"/>
+      <c r="BV35" s="10"/>
+      <c r="BW35" s="10"/>
       <c r="BX35" s="10"/>
-      <c r="BY35" s="10"/>
     </row>
-    <row r="36" spans="1:77" ht="12.5">
+    <row r="36" spans="1:76" ht="12.5">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="2"/>
@@ -3344,13 +3310,12 @@
       <c r="BR36" s="2"/>
       <c r="BS36" s="2"/>
       <c r="BT36" s="2"/>
-      <c r="BU36" s="2"/>
-      <c r="BV36" s="2"/>
-      <c r="BW36" s="9"/>
+      <c r="BU36" s="9"/>
+      <c r="BV36" s="10"/>
+      <c r="BW36" s="10"/>
       <c r="BX36" s="10"/>
-      <c r="BY36" s="10"/>
     </row>
-    <row r="37" spans="1:77" ht="12.5">
+    <row r="37" spans="1:76" ht="12.5">
       <c r="A37" s="2"/>
       <c r="B37" s="5"/>
       <c r="C37" s="2"/>
@@ -3423,24 +3388,23 @@
       <c r="BR37" s="2"/>
       <c r="BS37" s="2"/>
       <c r="BT37" s="2"/>
-      <c r="BU37" s="2"/>
-      <c r="BV37" s="2"/>
-      <c r="BW37" s="9"/>
+      <c r="BU37" s="9"/>
+      <c r="BV37" s="10"/>
+      <c r="BW37" s="10"/>
       <c r="BX37" s="10"/>
-      <c r="BY37" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:BX36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:BV36">
     <sortCondition ref="B5:B36"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="R3:AF3"/>
-    <mergeCell ref="AG3:AT3"/>
-    <mergeCell ref="AU3:BH3"/>
-    <mergeCell ref="BI3:BV3"/>
+    <mergeCell ref="C3:P3"/>
+    <mergeCell ref="Q3:AD3"/>
+    <mergeCell ref="AE3:AR3"/>
+    <mergeCell ref="AS3:BF3"/>
+    <mergeCell ref="BG3:BT3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>